<commit_message>
fix: updated file structure
</commit_message>
<xml_diff>
--- a/GroceryApp/src/main/resources/data.xlsx
+++ b/GroceryApp/src/main/resources/data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\reshm\eclipse-check\GroceryApp\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\reshm\git\checkGroceyApp\GroceryApp\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{399EBA7C-5E81-428D-AA30-0243B1CFCBC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07E37AAC-FDD9-4F99-A69A-F95A474E84B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,6 +22,10 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -341,25 +345,25 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="A1:C4"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" s="1">
+      <c r="A1">
         <v>111</v>
       </c>
-      <c r="B1" s="1">
-        <v>708</v>
+      <c r="B1">
+        <v>190</v>
       </c>
       <c r="C1" s="1"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" s="1">
+      <c r="A2">
         <v>123</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2">
         <v>324</v>
       </c>
       <c r="C2" s="1"/>

</xml_diff>